<commit_message>
3-runModel-cham more experiments stride 1
</commit_message>
<xml_diff>
--- a/ExperimentosGissella.xlsx
+++ b/ExperimentosGissella.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gissella_BejaranoNic\Documents\PeruvianSignLanguage\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31634CD1-B202-4EAE-90E8-F1AF944BA314}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EF60191-A213-4179-8C02-E6C254571623}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{B664CC47-0CDC-4C29-8327-B2D4CD6615DF}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="23">
   <si>
     <t>10nouns</t>
   </si>
@@ -60,9 +60,6 @@
     <t>DropOut</t>
   </si>
   <si>
-    <t>TestAcc</t>
-  </si>
-  <si>
     <t>e-5</t>
   </si>
   <si>
@@ -97,6 +94,15 @@
   </si>
   <si>
     <t>Chameleon</t>
+  </si>
+  <si>
+    <t>TestAcc (134 signs)</t>
+  </si>
+  <si>
+    <t>Comments</t>
+  </si>
+  <si>
+    <t>Analysis by sign and by subject</t>
   </si>
 </sst>
 </file>
@@ -112,12 +118,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -132,8 +144,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -448,11 +461,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98E7DA79-1D56-4C42-82B7-A2573CE01401}">
-  <dimension ref="A1:O25"/>
+  <dimension ref="A1:P25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F5" sqref="F5"/>
+      <selection pane="bottomLeft" activeCell="O6" sqref="O6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -462,15 +475,15 @@
     <col min="5" max="5" width="13.26953125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B1" t="s">
         <v>2</v>
       </c>
       <c r="C1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D1" t="s">
         <v>3</v>
@@ -485,33 +498,36 @@
         <v>6</v>
       </c>
       <c r="H1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I1" t="s">
         <v>17</v>
-      </c>
-      <c r="I1" t="s">
-        <v>18</v>
       </c>
       <c r="J1" t="s">
         <v>7</v>
       </c>
       <c r="K1" t="s">
+        <v>11</v>
+      </c>
+      <c r="L1" t="s">
         <v>12</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>13</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>14</v>
       </c>
-      <c r="N1" t="s">
-        <v>15</v>
-      </c>
       <c r="O1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.35">
+        <v>20</v>
+      </c>
+      <c r="P1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B2" t="s">
         <v>1</v>
@@ -523,7 +539,7 @@
         <v>20</v>
       </c>
       <c r="E2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F2">
         <v>40</v>
@@ -553,9 +569,9 @@
         <v>0.52170000000000005</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B3" t="s">
         <v>1</v>
@@ -567,7 +583,7 @@
         <v>16</v>
       </c>
       <c r="E3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F3">
         <v>40</v>
@@ -597,9 +613,9 @@
         <v>8.6999999999999994E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B4" t="s">
         <v>1</v>
@@ -611,7 +627,7 @@
         <v>20</v>
       </c>
       <c r="E4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F4">
         <v>40</v>
@@ -641,9 +657,9 @@
         <v>0.30430000000000001</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B5" t="s">
         <v>1</v>
@@ -655,7 +671,7 @@
         <v>20</v>
       </c>
       <c r="E5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F5">
         <v>100</v>
@@ -681,13 +697,16 @@
       <c r="M5">
         <v>0.99380000000000002</v>
       </c>
-      <c r="N5">
+      <c r="N5" s="1">
         <v>0.6522</v>
       </c>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="O5">
+        <v>0.23880000000000001</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B6" t="s">
         <v>1</v>
@@ -699,7 +718,7 @@
         <v>20</v>
       </c>
       <c r="E6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F6">
         <v>100</v>
@@ -729,9 +748,9 @@
         <v>0.52170000000000005</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B7" t="s">
         <v>1</v>
@@ -743,7 +762,7 @@
         <v>20</v>
       </c>
       <c r="E7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F7">
         <v>100</v>
@@ -773,9 +792,9 @@
         <v>0.30430000000000001</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B8" t="s">
         <v>1</v>
@@ -787,7 +806,7 @@
         <v>15</v>
       </c>
       <c r="E8" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F8">
         <v>100</v>
@@ -813,13 +832,16 @@
       <c r="M8">
         <v>0.93140000000000001</v>
       </c>
-      <c r="N8">
+      <c r="N8" s="1">
         <v>0.6522</v>
       </c>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="O8">
+        <v>0.37</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B9" t="s">
         <v>1</v>
@@ -831,7 +853,7 @@
         <v>15</v>
       </c>
       <c r="E9" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F9">
         <v>100</v>
@@ -861,9 +883,9 @@
         <v>0.56520000000000004</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B10" t="s">
         <v>1</v>
@@ -875,7 +897,7 @@
         <v>15</v>
       </c>
       <c r="E10" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F10">
         <v>100</v>
@@ -905,9 +927,9 @@
         <v>0.30430000000000001</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B11" t="s">
         <v>1</v>
@@ -919,7 +941,7 @@
         <v>10</v>
       </c>
       <c r="E11" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F11">
         <v>100</v>
@@ -945,13 +967,16 @@
       <c r="M11">
         <v>0.83130000000000004</v>
       </c>
-      <c r="N11">
+      <c r="N11" s="1">
         <v>0.69569999999999999</v>
       </c>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="O11">
+        <v>0.41</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B12" t="s">
         <v>1</v>
@@ -963,7 +988,7 @@
         <v>10</v>
       </c>
       <c r="E12" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F12">
         <v>100</v>
@@ -993,9 +1018,9 @@
         <v>0.52170000000000005</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B13" t="s">
         <v>1</v>
@@ -1007,7 +1032,7 @@
         <v>10</v>
       </c>
       <c r="E13" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F13">
         <v>100</v>
@@ -1037,9 +1062,9 @@
         <v>0.26090000000000002</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B14" t="s">
         <v>1</v>
@@ -1051,7 +1076,7 @@
         <v>10</v>
       </c>
       <c r="E14" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F14">
         <v>100</v>
@@ -1077,13 +1102,19 @@
       <c r="M14">
         <v>0.66900000000000004</v>
       </c>
-      <c r="N14">
+      <c r="N14" s="1">
         <v>0.82609999999999995</v>
       </c>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="O14">
+        <v>0.47</v>
+      </c>
+      <c r="P14" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B15" t="s">
         <v>1</v>
@@ -1095,7 +1126,7 @@
         <v>10</v>
       </c>
       <c r="E15" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F15">
         <v>100</v>
@@ -1125,9 +1156,9 @@
         <v>0.56520000000000004</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B16" t="s">
         <v>1</v>
@@ -1139,7 +1170,7 @@
         <v>10</v>
       </c>
       <c r="E16" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F16">
         <v>100</v>

</xml_diff>